<commit_message>
tree and graph gherkins with corresponding step definitions
</commit_message>
<xml_diff>
--- a/TestData/DSAlgo_Data_Driven_Testing.xlsx
+++ b/TestData/DSAlgo_Data_Driven_Testing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gayat\intellij-learning\SDET229Stars\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\SDETStars\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A65067-BF2A-46D1-838E-8A49A5FB90F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6632B1-830C-449A-9310-AD4078E4F435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{39EBA743-F911-448F-9B2B-80B78480DD9F}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="17280" windowHeight="10690" activeTab="1" xr2:uid="{39EBA743-F911-448F-9B2B-80B78480DD9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -112,10 +112,10 @@
     <t>SyntaxError: bad token T_OP on line 1</t>
   </si>
   <si>
+    <t>SyntaxError: EOF in multi-line statement on line 2</t>
+  </si>
+  <si>
     <t>((((((</t>
-  </si>
-  <si>
-    <t>SyntaxError: EOF in multi-line statement on line 2</t>
   </si>
 </sst>
 </file>
@@ -213,13 +213,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -239,9 +241,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -279,7 +281,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -385,7 +387,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -527,7 +529,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -648,10 +650,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{083714F2-18DE-4041-BAB2-2F243AD51ECB}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -662,87 +664,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="7"/>
+      <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6" t="s">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.35">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>12345</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.35">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Corrected codes in Tree, Graph,DS-Intro
</commit_message>
<xml_diff>
--- a/TestData/DSAlgo_Data_Driven_Testing.xlsx
+++ b/TestData/DSAlgo_Data_Driven_Testing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29725"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\SDETStars\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gayat\intellij-learning\SDET229Stars\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D24236-2C50-4360-A2CE-8D2B91043030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04722E78-7539-4A82-85B7-8F7CE8D33487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="14860" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -328,7 +328,7 @@
     <t>https://dsportalapp.herokuapp.com/graph/practice</t>
   </si>
   <si>
-    <t>https://dsportalapp.herokuapp.com/Tree/practice</t>
+    <t>https://dsportalapp.herokuapp.com/tree/practice</t>
   </si>
 </sst>
 </file>
@@ -835,8 +835,8 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1175,7 +1175,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.26953125" defaultRowHeight="14.25" customHeight="1"/>
@@ -1229,7 +1229,7 @@
       <c r="C4" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1240,7 +1240,7 @@
       <c r="C5" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1261,6 +1261,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D5" r:id="rId1" xr:uid="{D2FDE1DB-21AA-4F67-A14D-110CA1B1E11B}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{5DA5FF43-23BF-4646-BD3E-A74F2451E513}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1272,7 +1273,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.75" customHeight="1"/>

</xml_diff>